<commit_message>
Corrected reference to tables in the queries sheets of custom_beneficiaries and custom_individuals. Changed the required rows in the custom individuals form to only be custom_beneficiary_entity_row_id
</commit_message>
<xml_diff>
--- a/app/config/tables/custom_beneficiary_entities/forms/custom_beneficiary_entities/custom_beneficiary_entities.xlsx
+++ b/app/config/tables/custom_beneficiary_entities/forms/custom_beneficiary_entities/custom_beneficiary_entities.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/appGreece/config/tables/custom_beneficiary_entities/forms/custom_beneficiary_entities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/app/config/tables/custom_beneficiary_entities/forms/custom_beneficiary_entities/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19000" yWindow="3860" windowWidth="25600" windowHeight="16060" tabRatio="994" activeTab="1"/>
+    <workbookView xWindow="19000" yWindow="3860" windowWidth="25600" windowHeight="16060" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="171">
   <si>
     <t>clause</t>
   </si>
@@ -329,15 +329,6 @@
   </si>
   <si>
     <t>isSessionVariable</t>
-  </si>
-  <si>
-    <t>registrationMember</t>
-  </si>
-  <si>
-    <t>beneficiary_code = ?</t>
-  </si>
-  <si>
-    <t>[ data('beneficiary_code') ]</t>
   </si>
   <si>
     <t>Household Members Section:</t>
@@ -526,9 +517,6 @@
     <t>async_assign_single_string</t>
   </si>
   <si>
-    <t>{beneficiary_code: data('beneficiary_code'), _group_modify: metadata('_group_modify')}</t>
-  </si>
-  <si>
     <t>!data('tent_caravan')</t>
   </si>
   <si>
@@ -551,13 +539,49 @@
   </si>
   <si>
     <t>Custom Beneficiary Entities</t>
+  </si>
+  <si>
+    <t>custom_individuals</t>
+  </si>
+  <si>
+    <t>[ data('custom_beneficiary_entity_row_id')]</t>
+  </si>
+  <si>
+    <t>custom_beneficiary_entity_row_id = ?</t>
+  </si>
+  <si>
+    <t>{custom_beneficiary_entity_row_id: data('custom_beneficiary_entity_row_id'), _group_modify: metadata('_group_modify')}</t>
+  </si>
+  <si>
+    <r>
+      <t>[ data('</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>custom_beneficiary_entity_row_id'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>) ]</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -609,6 +633,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1266,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1321,7 +1351,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1355,7 +1385,7 @@
       <c r="E3" s="11"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -1374,7 +1404,7 @@
       <c r="E4" s="16"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
@@ -1400,13 +1430,13 @@
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -1533,10 +1563,10 @@
         <v>36</v>
       </c>
       <c r="K14" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="L14" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1545,17 +1575,17 @@
         <v>18</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F15" s="12"/>
       <c r="K15" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="L15" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1586,7 +1616,7 @@
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
@@ -1602,13 +1632,13 @@
         <v>94</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
@@ -1650,14 +1680,14 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F23" s="12"/>
       <c r="H23" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1683,7 +1713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1710,7 +1740,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C2"/>
     </row>
@@ -1728,7 +1758,7 @@
         <v>47</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C4"/>
     </row>
@@ -1737,7 +1767,7 @@
         <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1776,13 +1806,13 @@
         <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
         <v>52</v>
@@ -1796,16 +1826,16 @@
         <v>36</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -1816,16 +1846,16 @@
         <v>53</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -1836,16 +1866,16 @@
         <v>55</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -1856,16 +1886,16 @@
         <v>56</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -1876,16 +1906,16 @@
         <v>57</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -1896,16 +1926,16 @@
         <v>59</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -1916,16 +1946,16 @@
         <v>61</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -1936,16 +1966,16 @@
         <v>63</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -1956,16 +1986,16 @@
         <v>65</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2069,10 +2099,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2080,7 +2110,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2142,10 +2172,10 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2153,10 +2183,10 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2164,10 +2194,10 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2175,10 +2205,10 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2186,10 +2216,10 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2273,7 +2303,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2314,27 +2344,27 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>94</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>97</v>
+        <v>166</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>97</v>
+        <v>166</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>98</v>
+        <v>168</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>95</v>
@@ -2342,22 +2372,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>94</v>
       </c>
-      <c r="C3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" t="s">
-        <v>97</v>
+      <c r="C3" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>166</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>168</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
       <c r="G3" t="s">
         <v>95</v>
@@ -2438,7 +2468,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>2</v>
@@ -2446,7 +2476,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>27</v>
@@ -2454,7 +2484,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>27</v>
@@ -2462,7 +2492,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>27</v>
@@ -2470,7 +2500,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>27</v>
@@ -2478,7 +2508,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>27</v>
@@ -2486,7 +2516,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>27</v>
@@ -2494,7 +2524,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
enable/disable entitlements working. some new translations. add csvs to repo.
</commit_message>
<xml_diff>
--- a/app/config/tables/custom_beneficiary_entities/forms/custom_beneficiary_entities/custom_beneficiary_entities.xlsx
+++ b/app/config/tables/custom_beneficiary_entities/forms/custom_beneficiary_entities/custom_beneficiary_entities.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19000" yWindow="3860" windowWidth="25600" windowHeight="16060" tabRatio="994" activeTab="6"/>
+    <workbookView xWindow="16640" yWindow="4780" windowWidth="25600" windowHeight="16060" tabRatio="994" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="132">
   <si>
     <t>clause</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>text</t>
-  </si>
-  <si>
-    <t>text.spanish</t>
   </si>
   <si>
     <t>ID Number</t>
@@ -365,123 +362,6 @@
   </si>
   <si>
     <t>Athens</t>
-  </si>
-  <si>
-    <t>العنوان</t>
-  </si>
-  <si>
-    <t>نشانی</t>
-  </si>
-  <si>
-    <t>Dirección</t>
-  </si>
-  <si>
-    <t>رقم الهوية</t>
-  </si>
-  <si>
-    <t>شماره شناسایی</t>
-  </si>
-  <si>
-    <t>Número de ID</t>
-  </si>
-  <si>
-    <t>المدينة</t>
-  </si>
-  <si>
-    <t>شهر</t>
-  </si>
-  <si>
-    <t>Ciudad</t>
-  </si>
-  <si>
-    <t>رقم التليفون</t>
-  </si>
-  <si>
-    <t>تلفن</t>
-  </si>
-  <si>
-    <t>Teléfono</t>
-  </si>
-  <si>
-    <t>شركة الموبايل</t>
-  </si>
-  <si>
-    <t>ارائه دهنده تلفن همراه</t>
-  </si>
-  <si>
-    <t>Proveedor móvil</t>
-  </si>
-  <si>
-    <t>تم تمكينها بنجاح</t>
-  </si>
-  <si>
-    <t>موفقیت فعال!</t>
-  </si>
-  <si>
-    <t>Activado satisfactoriamente!</t>
-  </si>
-  <si>
-    <t>تم تعطيلها بنجاح</t>
-  </si>
-  <si>
-    <t>موفقیت غیر فعال!</t>
-  </si>
-  <si>
-    <t>Desactivado satisfactoriamente!</t>
-  </si>
-  <si>
-    <t>اختيار اتحقاق للتسليم</t>
-  </si>
-  <si>
-    <t xml:space="preserve">انتخاب  به عنوان حق برای ارائه </t>
-  </si>
-  <si>
-    <t>Elegir un título para distribuir</t>
-  </si>
-  <si>
-    <t>لا استحقاقات للتسليم</t>
-  </si>
-  <si>
-    <t xml:space="preserve">تحویل بدون به  حقوق </t>
-  </si>
-  <si>
-    <t>No hay títulos para entregar</t>
-  </si>
-  <si>
-    <t>text.arabic</t>
-  </si>
-  <si>
-    <t>text.farsi</t>
-  </si>
-  <si>
-    <t>Διεύθυνση</t>
-  </si>
-  <si>
-    <t>Αριθμό ταυτότητας</t>
-  </si>
-  <si>
-    <t>Πόλη</t>
-  </si>
-  <si>
-    <t>Τηλέφωνο</t>
-  </si>
-  <si>
-    <t>Παροχέας κινητής τηλεφωνίας</t>
-  </si>
-  <si>
-    <t>Επιτυχής!</t>
-  </si>
-  <si>
-    <t>Επιτυχής Απενεργοποίηση!</t>
-  </si>
-  <si>
-    <t>Επιλέξτε ένα Δικαίωμα παράδοσης</t>
-  </si>
-  <si>
-    <t>Δεν υπάρχουν Δικαιώματα παράδοσης</t>
-  </si>
-  <si>
-    <t>text.greek</t>
   </si>
   <si>
     <t>async_assign_count</t>
@@ -564,12 +444,27 @@
   <si>
     <t>{custom_beneficiary_entity_row_id: metadata('_id'), _group_modify: metadata('_group_modify')}</t>
   </si>
+  <si>
+    <t>Delivery Site</t>
+  </si>
+  <si>
+    <t>Household Size</t>
+  </si>
+  <si>
+    <t>Disabled Reason</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Tent/Caravan Code</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -612,13 +507,6 @@
       <sz val="12"/>
       <color theme="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -779,7 +667,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -832,8 +720,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -1337,8 +1223,8 @@
       <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="36" t="s">
-        <v>158</v>
+      <c r="L1" s="34" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1379,13 +1265,13 @@
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="33" t="s">
         <v>101</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>102</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
@@ -1512,10 +1398,10 @@
         <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="L12" t="s">
-        <v>159</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1524,17 +1410,17 @@
         <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="F13" s="12"/>
       <c r="K13" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="L13" t="s">
-        <v>159</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1565,7 +1451,7 @@
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -1578,16 +1464,16 @@
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>97</v>
-      </c>
       <c r="H17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -1629,14 +1515,14 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F21" s="12"/>
       <c r="H21" s="1" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1689,7 +1575,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="C2"/>
     </row>
@@ -1707,7 +1593,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="C4"/>
     </row>
@@ -1716,7 +1602,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1735,216 +1621,136 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="3" width="41" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F5" s="34" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>56</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F7" s="34" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>58</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" s="34" t="s">
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>127</v>
       </c>
-      <c r="F8" s="34" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" s="34" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="34" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
         <v>130</v>
       </c>
-      <c r="F9" s="34" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="E10" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1958,7 +1764,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1976,7 +1782,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2024,7 +1830,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2048,10 +1854,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2059,7 +1865,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2085,10 +1891,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>70</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>71</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>42</v>
@@ -2099,10 +1905,10 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2110,10 +1916,10 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2121,10 +1927,10 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2132,10 +1938,10 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2143,10 +1949,10 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2154,10 +1960,10 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2165,10 +1971,10 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2192,13 +1998,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>75</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>76</v>
       </c>
       <c r="D1" s="25" t="s">
         <v>2</v>
@@ -2209,36 +2015,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>78</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>79</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" t="s">
-        <v>78</v>
-      </c>
       <c r="C3" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
         <v>81</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="25" t="s">
         <v>82</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2251,7 +2057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2269,80 +2075,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>90</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="E3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F3" t="s">
-        <v>164</v>
-      </c>
-      <c r="G3" t="s">
-        <v>93</v>
-      </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2373,27 +2179,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>65</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2417,7 +2223,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>2</v>
@@ -2425,7 +2231,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>25</v>
@@ -2433,7 +2239,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>25</v>
@@ -2441,7 +2247,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>25</v>
@@ -2449,7 +2255,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>25</v>
@@ -2457,7 +2263,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>25</v>
@@ -2465,7 +2271,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>25</v>
@@ -2473,7 +2279,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
final changes for demo screenshots. include tables.init. Hardcoding is only temporary fix.
</commit_message>
<xml_diff>
--- a/app/config/tables/custom_beneficiary_entities/forms/custom_beneficiary_entities/custom_beneficiary_entities.xlsx
+++ b/app/config/tables/custom_beneficiary_entities/forms/custom_beneficiary_entities/custom_beneficiary_entities.xlsx
@@ -187,9 +187,6 @@
     <t>string_token</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>ID Number</t>
   </si>
   <si>
@@ -458,6 +455,9 @@
   </si>
   <si>
     <t>Tent/Caravan Code</t>
+  </si>
+  <si>
+    <t>text.default</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1224,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1265,13 +1265,13 @@
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="33" t="s">
         <v>100</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>101</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
@@ -1398,10 +1398,10 @@
         <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1410,17 +1410,17 @@
         <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="F13" s="12"/>
       <c r="K13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -1464,16 +1464,16 @@
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>96</v>
-      </c>
       <c r="H17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -1515,14 +1515,14 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F21" s="12"/>
       <c r="H21" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1575,7 +1575,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2"/>
     </row>
@@ -1593,7 +1593,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4"/>
     </row>
@@ -1602,7 +1602,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1624,7 +1624,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1638,7 +1638,7 @@
         <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1654,15 +1654,15 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
         <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1670,7 +1670,7 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1678,39 +1678,39 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
         <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
         <v>57</v>
-      </c>
-      <c r="B8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
         <v>59</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
         <v>61</v>
-      </c>
-      <c r="B10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1718,7 +1718,7 @@
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1726,15 +1726,15 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1742,15 +1742,15 @@
         <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1782,7 +1782,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1830,7 +1830,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1854,10 +1854,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1865,7 +1865,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1891,10 +1891,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>70</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>42</v>
@@ -1905,10 +1905,10 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1916,10 +1916,10 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1927,10 +1927,10 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1938,10 +1938,10 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1949,10 +1949,10 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1960,10 +1960,10 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1971,10 +1971,10 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1998,13 +1998,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>75</v>
       </c>
       <c r="D1" s="25" t="s">
         <v>2</v>
@@ -2015,36 +2015,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>77</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>78</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" t="s">
-        <v>77</v>
-      </c>
       <c r="C3" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
         <v>80</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="25" t="s">
         <v>81</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2075,80 +2075,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>89</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>91</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G3" t="s">
-        <v>92</v>
-      </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2179,27 +2179,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>64</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2223,7 +2223,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>2</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>25</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>25</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>25</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>25</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>25</v>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>25</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
fix reg detail view if in individual mode
</commit_message>
<xml_diff>
--- a/app/config/tables/custom_beneficiary_entities/forms/custom_beneficiary_entities/custom_beneficiary_entities.xlsx
+++ b/app/config/tables/custom_beneficiary_entities/forms/custom_beneficiary_entities/custom_beneficiary_entities.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10420" yWindow="4820" windowWidth="25600" windowHeight="16060" tabRatio="994" activeTab="3"/>
+    <workbookView xWindow="10420" yWindow="4820" windowWidth="25600" windowHeight="16060" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="initial" sheetId="11" r:id="rId7"/>
     <sheet name="prompt_types" sheetId="12" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1104,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1230,15 +1230,19 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="12"/>
+        <v>19</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="H6"/>
       <c r="I6"/>
-      <c r="J6"/>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
       <c r="K6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1248,19 +1252,15 @@
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F7" s="12"/>
       <c r="H7"/>
       <c r="I7"/>
-      <c r="J7" t="s">
-        <v>21</v>
-      </c>
+      <c r="J7"/>
       <c r="K7"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1283,20 +1283,22 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="H10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" t="b">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1305,16 +1307,14 @@
         <v>13</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F11" s="12"/>
       <c r="K11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L11" t="s">
         <v>100</v>
@@ -1323,20 +1323,20 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="F12" s="12"/>
-      <c r="K12" t="s">
-        <v>98</v>
-      </c>
-      <c r="L12" t="s">
-        <v>100</v>
+      <c r="H12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1654,7 +1654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>